<commit_message>
includes option 'other...' for bait set
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.15.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.15.balsamic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB2D680-58E7-4441-BB69-6F6B1209A3D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55DBC85-D50B-E54A-952B-BBF356766EF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4620" yWindow="2640" windowWidth="41060" windowHeight="21100" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="449">
   <si>
     <t>&lt;TABLE HEADER&gt;</t>
   </si>
@@ -1820,6 +1820,9 @@
   </si>
   <si>
     <t>tumour-purity-test-2</t>
+  </si>
+  <si>
+    <t>other (specify in comment field)</t>
   </si>
 </sst>
 </file>
@@ -3231,6 +3234,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3273,7 +3277,6 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="334">
     <cellStyle name="Excel Built-in Normal" xfId="45" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -4096,7 +4099,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4140,7 +4143,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="000000">
@@ -4502,7 +4505,7 @@
   <dimension ref="A1:AC428"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A34"/>
+      <selection activeCell="U19" sqref="U19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -4778,47 +4781,47 @@
       <c r="AC8" s="99"/>
     </row>
     <row r="9" spans="1:29" s="105" customFormat="1" ht="22" customHeight="1" outlineLevel="1">
-      <c r="A9" s="177" t="s">
+      <c r="A9" s="178" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="178"/>
-      <c r="C9" s="178"/>
-      <c r="D9" s="178"/>
-      <c r="E9" s="178"/>
-      <c r="F9" s="178"/>
-      <c r="G9" s="178"/>
-      <c r="H9" s="178"/>
-      <c r="I9" s="178"/>
-      <c r="J9" s="178"/>
-      <c r="K9" s="179"/>
+      <c r="B9" s="179"/>
+      <c r="C9" s="179"/>
+      <c r="D9" s="179"/>
+      <c r="E9" s="179"/>
+      <c r="F9" s="179"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="179"/>
+      <c r="I9" s="179"/>
+      <c r="J9" s="179"/>
+      <c r="K9" s="180"/>
       <c r="L9" s="101"/>
-      <c r="M9" s="180" t="s">
+      <c r="M9" s="181" t="s">
         <v>105</v>
       </c>
-      <c r="N9" s="181"/>
+      <c r="N9" s="182"/>
       <c r="O9" s="102"/>
-      <c r="P9" s="183" t="s">
+      <c r="P9" s="184" t="s">
         <v>374</v>
       </c>
-      <c r="Q9" s="184"/>
-      <c r="R9" s="184"/>
-      <c r="S9" s="185"/>
+      <c r="Q9" s="185"/>
+      <c r="R9" s="185"/>
+      <c r="S9" s="186"/>
       <c r="T9" s="103"/>
-      <c r="U9" s="189" t="s">
+      <c r="U9" s="190" t="s">
         <v>363</v>
       </c>
-      <c r="V9" s="190"/>
+      <c r="V9" s="191"/>
       <c r="W9" s="104"/>
-      <c r="X9" s="186" t="s">
+      <c r="X9" s="187" t="s">
         <v>375</v>
       </c>
-      <c r="Y9" s="187"/>
-      <c r="Z9" s="188"/>
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="189"/>
       <c r="AA9" s="103"/>
-      <c r="AB9" s="182" t="s">
+      <c r="AB9" s="183" t="s">
         <v>207</v>
       </c>
-      <c r="AC9" s="182"/>
+      <c r="AC9" s="183"/>
     </row>
     <row r="10" spans="1:29" s="105" customFormat="1" ht="13" hidden="1" customHeight="1">
       <c r="A10" s="106" t="s">
@@ -5191,7 +5194,7 @@
       <c r="R16" s="62"/>
       <c r="S16" s="63"/>
       <c r="T16" s="157"/>
-      <c r="U16" s="191" t="s">
+      <c r="U16" s="177" t="s">
         <v>441</v>
       </c>
       <c r="V16">
@@ -5365,7 +5368,7 @@
       <c r="S19" s="63"/>
       <c r="T19" s="157"/>
       <c r="U19" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="V19">
         <v>25</v>

</xml_diff>

<commit_message>
adds real 1508:15 orderforms
</commit_message>
<xml_diff>
--- a/tests/fixtures/orderforms/1508.15.balsamic.xlsx
+++ b/tests/fixtures/orderforms/1508.15.balsamic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrikgrenfeldt/Documents/src/cg/tests/fixtures/orderforms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55DBC85-D50B-E54A-952B-BBF356766EF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BE6990A-E362-CB45-A114-175EDDA87E7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4620" yWindow="2640" windowWidth="41060" windowHeight="21100" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1600" yWindow="460" windowWidth="34140" windowHeight="20920" tabRatio="262" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="information" sheetId="5" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <definedName name="description" localSheetId="2">'Drop down lists'!$C$21</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1335,9 +1336,6 @@
       <t xml:space="preserve">the sample id of the father
 </t>
     </r>
-  </si>
-  <si>
-    <t xml:space="preserve">1508:14 Orderform </t>
   </si>
   <si>
     <r>
@@ -1685,9 +1683,6 @@
     <t>CSP</t>
   </si>
   <si>
-    <t>Emilia Ottosson Laakso</t>
-  </si>
-  <si>
     <t>Valtteri Wirta</t>
   </si>
   <si>
@@ -1726,75 +1721,87 @@
     <t>muscle</t>
   </si>
   <si>
+    <t xml:space="preserve">1508:15 Orderform </t>
+  </si>
+  <si>
+    <t>Anna Gellerbring</t>
+  </si>
+  <si>
+    <t>whole-genome-1</t>
+  </si>
+  <si>
+    <t>whole-genome</t>
+  </si>
+  <si>
+    <t>plate</t>
+  </si>
+  <si>
+    <t>whole-genome-2</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>whole-genome-3</t>
+  </si>
+  <si>
+    <t>whole-genome-4</t>
+  </si>
+  <si>
+    <t>whole-genome-5</t>
+  </si>
+  <si>
+    <t>whole-genome-6</t>
+  </si>
+  <si>
+    <t>whole-genome-7</t>
+  </si>
+  <si>
+    <t>whole-genome-8</t>
+  </si>
+  <si>
+    <t>whole-genome-9</t>
+  </si>
+  <si>
+    <t>whole-genome-10</t>
+  </si>
+  <si>
+    <t>whole-exome-1</t>
+  </si>
+  <si>
+    <t>whole-exome</t>
+  </si>
+  <si>
+    <t>whole-exome-2</t>
+  </si>
+  <si>
+    <t>whole-exome-3</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-1</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-2</t>
+  </si>
+  <si>
+    <t>cancer-capture-panels-3</t>
+  </si>
+  <si>
+    <t>rna-1</t>
+  </si>
+  <si>
     <t>rna</t>
   </si>
   <si>
-    <t>plate</t>
-  </si>
-  <si>
-    <t>whole-genome</t>
-  </si>
-  <si>
-    <t>whole-exome</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels</t>
-  </si>
-  <si>
-    <t>whole-genome-1</t>
-  </si>
-  <si>
-    <t>whole-genome-2</t>
-  </si>
-  <si>
-    <t>whole-genome-3</t>
-  </si>
-  <si>
-    <t>whole-genome-4</t>
-  </si>
-  <si>
-    <t>whole-genome-5</t>
-  </si>
-  <si>
-    <t>whole-genome-6</t>
-  </si>
-  <si>
-    <t>whole-genome-7</t>
-  </si>
-  <si>
-    <t>whole-genome-8</t>
-  </si>
-  <si>
-    <t>whole-genome-9</t>
-  </si>
-  <si>
-    <t>whole-genome-10</t>
-  </si>
-  <si>
-    <t>whole-exome-1</t>
-  </si>
-  <si>
-    <t>whole-exome-2</t>
-  </si>
-  <si>
-    <t>whole-exome-3</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-1</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-2</t>
-  </si>
-  <si>
-    <t>cancer-capture-panels-3</t>
-  </si>
-  <si>
-    <t>rna-1</t>
-  </si>
-  <si>
     <t>rna-2</t>
   </si>
   <si>
+    <t>comment</t>
+  </si>
+  <si>
     <t>gene-list-test</t>
   </si>
   <si>
@@ -1810,19 +1817,13 @@
     <t>GMSmyeloid</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>comment</t>
+    <t>other (specify in comment field)</t>
   </si>
   <si>
     <t>tumour-purity-test-1</t>
   </si>
   <si>
     <t>tumour-purity-test-2</t>
-  </si>
-  <si>
-    <t>other (specify in comment field)</t>
   </si>
 </sst>
 </file>
@@ -3234,7 +3235,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="44" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3277,6 +3277,7 @@
     <xf numFmtId="0" fontId="12" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="334">
     <cellStyle name="Excel Built-in Normal" xfId="45" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -3707,7 +3708,7 @@
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>2310553</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>55034</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4167,8 +4168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A7" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection sqref="A1:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -4185,7 +4186,7 @@
         <v>22</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>371</v>
+        <v>414</v>
       </c>
       <c r="D1" s="9"/>
       <c r="E1" s="2"/>
@@ -4203,7 +4204,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>409</v>
+        <v>415</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>24</v>
@@ -4218,7 +4219,7 @@
         <v>25</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>26</v>
@@ -4229,7 +4230,6 @@
     </row>
     <row r="5" spans="1:5" hidden="1"/>
     <row r="6" spans="1:5" hidden="1"/>
-    <row r="7" spans="1:5" hidden="1"/>
     <row r="14" spans="1:5" ht="19">
       <c r="A14" s="41" t="s">
         <v>250</v>
@@ -4242,27 +4242,27 @@
     </row>
     <row r="16" spans="1:5" ht="14">
       <c r="A16" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="14">
       <c r="A17" s="16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="14">
       <c r="A18" s="16" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="14">
       <c r="A19" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="14">
       <c r="A20" s="16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="16">
@@ -4282,12 +4282,12 @@
     </row>
     <row r="26" spans="1:1" ht="28">
       <c r="A26" s="36" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="98">
       <c r="A27" s="36" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="36" customHeight="1">
@@ -4302,7 +4302,7 @@
     </row>
     <row r="30" spans="1:1" ht="27" customHeight="1">
       <c r="A30" s="36" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="28">
@@ -4317,7 +4317,7 @@
     </row>
     <row r="33" spans="1:5" ht="52" customHeight="1">
       <c r="A33" s="35" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C33" s="16"/>
       <c r="E33" s="16"/>
@@ -4396,32 +4396,32 @@
     </row>
     <row r="51" spans="1:1" ht="28">
       <c r="A51" s="35" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="14">
       <c r="A52" s="35" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="54" spans="1:1">
       <c r="A54" s="20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="14">
       <c r="A56" s="35" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="28" customHeight="1">
       <c r="A57" s="37" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="28" customHeight="1">
       <c r="A58" s="37" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="59" spans="1:1">
@@ -4482,7 +4482,7 @@
       <c r="A80" s="16"/>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="YC2FrqvxuxCdgPs2rz0v2G7WVpDLnlfsPKGuUC3HUIoAOtq1+GH3+sQFpGgKkaMWpQuALORguIp/pjneAcENiQ==" saltValue="xSK47VJfeSLePxG37PQCnw==" spinCount="100000" sheet="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <hyperlinks>
     <hyperlink ref="A14" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
@@ -4504,8 +4504,8 @@
   </sheetPr>
   <dimension ref="A1:AC428"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.6640625" defaultRowHeight="13" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -4513,7 +4513,7 @@
     <col min="1" max="1" width="18" style="71" customWidth="1"/>
     <col min="2" max="2" width="8" style="165" customWidth="1"/>
     <col min="3" max="3" width="7.83203125" style="166" customWidth="1"/>
-    <col min="4" max="4" width="21.83203125" style="165" customWidth="1"/>
+    <col min="4" max="4" width="8.5" style="165" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" style="167" customWidth="1"/>
     <col min="6" max="6" width="6.1640625" style="71" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" style="71"/>
@@ -4781,47 +4781,47 @@
       <c r="AC8" s="99"/>
     </row>
     <row r="9" spans="1:29" s="105" customFormat="1" ht="22" customHeight="1" outlineLevel="1">
-      <c r="A9" s="178" t="s">
+      <c r="A9" s="177" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="179"/>
-      <c r="C9" s="179"/>
-      <c r="D9" s="179"/>
-      <c r="E9" s="179"/>
-      <c r="F9" s="179"/>
-      <c r="G9" s="179"/>
-      <c r="H9" s="179"/>
-      <c r="I9" s="179"/>
-      <c r="J9" s="179"/>
-      <c r="K9" s="180"/>
+      <c r="B9" s="178"/>
+      <c r="C9" s="178"/>
+      <c r="D9" s="178"/>
+      <c r="E9" s="178"/>
+      <c r="F9" s="178"/>
+      <c r="G9" s="178"/>
+      <c r="H9" s="178"/>
+      <c r="I9" s="178"/>
+      <c r="J9" s="178"/>
+      <c r="K9" s="179"/>
       <c r="L9" s="101"/>
-      <c r="M9" s="181" t="s">
+      <c r="M9" s="180" t="s">
         <v>105</v>
       </c>
-      <c r="N9" s="182"/>
+      <c r="N9" s="181"/>
       <c r="O9" s="102"/>
-      <c r="P9" s="184" t="s">
+      <c r="P9" s="183" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q9" s="184"/>
+      <c r="R9" s="184"/>
+      <c r="S9" s="185"/>
+      <c r="T9" s="103"/>
+      <c r="U9" s="189" t="s">
+        <v>363</v>
+      </c>
+      <c r="V9" s="190"/>
+      <c r="W9" s="104"/>
+      <c r="X9" s="186" t="s">
         <v>374</v>
       </c>
-      <c r="Q9" s="185"/>
-      <c r="R9" s="185"/>
-      <c r="S9" s="186"/>
-      <c r="T9" s="103"/>
-      <c r="U9" s="190" t="s">
-        <v>363</v>
-      </c>
-      <c r="V9" s="191"/>
-      <c r="W9" s="104"/>
-      <c r="X9" s="187" t="s">
-        <v>375</v>
-      </c>
-      <c r="Y9" s="188"/>
-      <c r="Z9" s="189"/>
+      <c r="Y9" s="187"/>
+      <c r="Z9" s="188"/>
       <c r="AA9" s="103"/>
-      <c r="AB9" s="183" t="s">
+      <c r="AB9" s="182" t="s">
         <v>207</v>
       </c>
-      <c r="AC9" s="183"/>
+      <c r="AC9" s="182"/>
     </row>
     <row r="10" spans="1:29" s="105" customFormat="1" ht="13" hidden="1" customHeight="1">
       <c r="A10" s="106" t="s">
@@ -4919,13 +4919,13 @@
       </c>
       <c r="W11" s="122"/>
       <c r="X11" s="121" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="Y11" s="121" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="Z11" s="121" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="AA11" s="123"/>
       <c r="AB11" s="109" t="s">
@@ -5024,20 +5024,20 @@
       </c>
       <c r="T13" s="145"/>
       <c r="U13" s="141" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="V13" s="147" t="s">
         <v>307</v>
       </c>
       <c r="W13" s="148"/>
       <c r="X13" s="146" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="Y13" s="149" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z13" s="149" t="s">
         <v>385</v>
-      </c>
-      <c r="Z13" s="149" t="s">
-        <v>386</v>
       </c>
       <c r="AA13" s="150"/>
       <c r="AB13" s="117" t="s">
@@ -5082,7 +5082,7 @@
     </row>
     <row r="15" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A15" s="58" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="B15" s="56" t="s">
         <v>37</v>
@@ -5094,7 +5094,7 @@
         <v>289</v>
       </c>
       <c r="E15" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F15" s="57" t="s">
         <v>15</v>
@@ -5116,7 +5116,7 @@
       </c>
       <c r="L15" s="156"/>
       <c r="M15" s="61" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="N15" s="60" t="s">
         <v>27</v>
@@ -5128,7 +5128,7 @@
       <c r="S15" s="58"/>
       <c r="T15" s="157"/>
       <c r="U15" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="V15">
         <v>5</v>
@@ -5141,19 +5141,19 @@
         <v>2</v>
       </c>
       <c r="Z15" s="66" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="AA15" s="159"/>
       <c r="AB15" s="61" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
       <c r="AC15" s="61" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A16" s="58" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B16" s="56" t="s">
         <v>37</v>
@@ -5165,7 +5165,7 @@
         <v>290</v>
       </c>
       <c r="E16" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F16" s="57" t="s">
         <v>16</v>
@@ -5194,8 +5194,8 @@
       <c r="R16" s="62"/>
       <c r="S16" s="63"/>
       <c r="T16" s="157"/>
-      <c r="U16" s="177" t="s">
-        <v>441</v>
+      <c r="U16" s="191" t="s">
+        <v>443</v>
       </c>
       <c r="V16">
         <v>10</v>
@@ -5204,7 +5204,7 @@
       <c r="X16" s="65"/>
       <c r="Y16" s="65"/>
       <c r="Z16" s="66" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="AA16" s="159"/>
       <c r="AB16" s="61"/>
@@ -5212,7 +5212,7 @@
     </row>
     <row r="17" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A17" s="58" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B17" s="56" t="s">
         <v>37</v>
@@ -5224,7 +5224,7 @@
         <v>291</v>
       </c>
       <c r="E17" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F17" s="57" t="s">
         <v>15</v>
@@ -5254,7 +5254,7 @@
       <c r="S17" s="63"/>
       <c r="T17" s="157"/>
       <c r="U17" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="V17">
         <v>15</v>
@@ -5269,7 +5269,7 @@
     </row>
     <row r="18" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A18" s="58" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B18" s="56" t="s">
         <v>37</v>
@@ -5281,7 +5281,7 @@
         <v>292</v>
       </c>
       <c r="E18" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F18" s="57" t="s">
         <v>77</v>
@@ -5311,7 +5311,7 @@
       <c r="S18" s="63"/>
       <c r="T18" s="157"/>
       <c r="U18" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V18">
         <v>20</v>
@@ -5326,7 +5326,7 @@
     </row>
     <row r="19" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A19" s="58" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B19" s="56" t="s">
         <v>37</v>
@@ -5338,7 +5338,7 @@
         <v>293</v>
       </c>
       <c r="E19" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F19" s="57" t="s">
         <v>77</v>
@@ -5347,7 +5347,7 @@
         <v>94</v>
       </c>
       <c r="H19" s="42" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I19" s="21" t="s">
         <v>103</v>
@@ -5368,7 +5368,7 @@
       <c r="S19" s="63"/>
       <c r="T19" s="157"/>
       <c r="U19" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="V19">
         <v>25</v>
@@ -5383,7 +5383,7 @@
     </row>
     <row r="20" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A20" s="58" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B20" s="56" t="s">
         <v>37</v>
@@ -5395,7 +5395,7 @@
         <v>294</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F20" s="57" t="s">
         <v>77</v>
@@ -5425,7 +5425,7 @@
       <c r="S20" s="63"/>
       <c r="T20" s="157"/>
       <c r="U20" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V20">
         <v>30</v>
@@ -5440,7 +5440,7 @@
     </row>
     <row r="21" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A21" s="58" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B21" s="56" t="s">
         <v>37</v>
@@ -5452,7 +5452,7 @@
         <v>295</v>
       </c>
       <c r="E21" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F21" s="57" t="s">
         <v>77</v>
@@ -5482,7 +5482,7 @@
       <c r="S21" s="63"/>
       <c r="T21" s="157"/>
       <c r="U21" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V21">
         <v>35</v>
@@ -5497,7 +5497,7 @@
     </row>
     <row r="22" spans="1:29" s="133" customFormat="1" ht="25" customHeight="1">
       <c r="A22" s="58" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B22" s="56" t="s">
         <v>37</v>
@@ -5509,7 +5509,7 @@
         <v>296</v>
       </c>
       <c r="E22" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F22" s="57" t="s">
         <v>77</v>
@@ -5539,7 +5539,7 @@
       <c r="S22" s="63"/>
       <c r="T22" s="157"/>
       <c r="U22" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V22">
         <v>40</v>
@@ -5554,7 +5554,7 @@
     </row>
     <row r="23" spans="1:29" ht="25" customHeight="1">
       <c r="A23" s="58" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B23" s="56" t="s">
         <v>37</v>
@@ -5566,7 +5566,7 @@
         <v>297</v>
       </c>
       <c r="E23" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F23" s="57" t="s">
         <v>77</v>
@@ -5596,7 +5596,7 @@
       <c r="S23" s="63"/>
       <c r="T23" s="157"/>
       <c r="U23" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V23">
         <v>45</v>
@@ -5611,7 +5611,7 @@
     </row>
     <row r="24" spans="1:29" ht="25" customHeight="1">
       <c r="A24" s="58" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B24" s="56" t="s">
         <v>37</v>
@@ -5623,7 +5623,7 @@
         <v>298</v>
       </c>
       <c r="E24" s="58" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="F24" s="57" t="s">
         <v>77</v>
@@ -5632,7 +5632,7 @@
         <v>94</v>
       </c>
       <c r="H24" s="176" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I24" s="21" t="s">
         <v>103</v>
@@ -5653,7 +5653,7 @@
       <c r="S24" s="63"/>
       <c r="T24" s="157"/>
       <c r="U24" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V24">
         <v>50</v>
@@ -5668,7 +5668,7 @@
     </row>
     <row r="25" spans="1:29" ht="25" customHeight="1">
       <c r="A25" s="58" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B25" s="56" t="s">
         <v>37</v>
@@ -5680,7 +5680,7 @@
         <v>285</v>
       </c>
       <c r="E25" s="58" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="F25" s="57" t="s">
         <v>77</v>
@@ -5689,7 +5689,7 @@
         <v>94</v>
       </c>
       <c r="H25" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I25" s="21" t="s">
         <v>103</v>
@@ -5710,7 +5710,7 @@
       <c r="S25" s="63"/>
       <c r="T25" s="157"/>
       <c r="U25" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V25">
         <v>55</v>
@@ -5725,7 +5725,7 @@
     </row>
     <row r="26" spans="1:29" ht="25" customHeight="1">
       <c r="A26" s="58" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B26" s="56" t="s">
         <v>37</v>
@@ -5734,10 +5734,10 @@
         <v>310</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E26" s="58" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="F26" s="57" t="s">
         <v>77</v>
@@ -5767,7 +5767,7 @@
       <c r="S26" s="63"/>
       <c r="T26" s="157"/>
       <c r="U26" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V26">
         <v>60</v>
@@ -5782,7 +5782,7 @@
     </row>
     <row r="27" spans="1:29" s="160" customFormat="1" ht="25" customHeight="1">
       <c r="A27" s="58" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B27" s="56" t="s">
         <v>37</v>
@@ -5791,10 +5791,10 @@
         <v>310</v>
       </c>
       <c r="D27" s="53" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="E27" s="58" t="s">
-        <v>419</v>
+        <v>430</v>
       </c>
       <c r="F27" s="57" t="s">
         <v>77</v>
@@ -5803,7 +5803,7 @@
         <v>94</v>
       </c>
       <c r="H27" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I27" s="21" t="s">
         <v>103</v>
@@ -5824,7 +5824,7 @@
       <c r="S27" s="63"/>
       <c r="T27" s="157"/>
       <c r="U27" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V27">
         <v>65</v>
@@ -5839,7 +5839,7 @@
     </row>
     <row r="28" spans="1:29" s="160" customFormat="1" ht="25" customHeight="1">
       <c r="A28" s="58" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B28" s="56" t="s">
         <v>37</v>
@@ -5848,10 +5848,10 @@
         <v>310</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E28" s="58" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="F28" s="57" t="s">
         <v>77</v>
@@ -5860,7 +5860,7 @@
         <v>94</v>
       </c>
       <c r="H28" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I28" s="21" t="s">
         <v>103</v>
@@ -5881,7 +5881,7 @@
       <c r="S28" s="63"/>
       <c r="T28" s="157"/>
       <c r="U28" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V28">
         <v>70</v>
@@ -5908,7 +5908,7 @@
         <v>251</v>
       </c>
       <c r="E29" s="58" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="F29" s="57" t="s">
         <v>77</v>
@@ -5917,7 +5917,7 @@
         <v>94</v>
       </c>
       <c r="H29" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I29" s="21" t="s">
         <v>103</v>
@@ -5938,7 +5938,7 @@
       <c r="S29" s="63"/>
       <c r="T29" s="157"/>
       <c r="U29" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V29">
         <v>75</v>
@@ -5962,10 +5962,10 @@
         <v>310</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E30" s="58" t="s">
-        <v>420</v>
+        <v>434</v>
       </c>
       <c r="F30" s="57" t="s">
         <v>77</v>
@@ -5974,7 +5974,7 @@
         <v>94</v>
       </c>
       <c r="H30" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I30" s="21" t="s">
         <v>103</v>
@@ -5995,7 +5995,7 @@
       <c r="S30" s="63"/>
       <c r="T30" s="157"/>
       <c r="U30" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V30">
         <v>80</v>
@@ -6022,7 +6022,7 @@
         <v>300</v>
       </c>
       <c r="E31" s="58" t="s">
-        <v>416</v>
+        <v>438</v>
       </c>
       <c r="F31" s="57" t="s">
         <v>77</v>
@@ -6031,7 +6031,7 @@
         <v>94</v>
       </c>
       <c r="H31" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I31" s="21" t="s">
         <v>103</v>
@@ -6052,7 +6052,7 @@
       <c r="S31" s="63"/>
       <c r="T31" s="157"/>
       <c r="U31" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V31">
         <v>85</v>
@@ -6067,7 +6067,7 @@
     </row>
     <row r="32" spans="1:29" s="160" customFormat="1" ht="25" customHeight="1">
       <c r="A32" s="58" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="B32" s="56" t="s">
         <v>37</v>
@@ -6079,7 +6079,7 @@
         <v>301</v>
       </c>
       <c r="E32" s="58" t="s">
-        <v>416</v>
+        <v>438</v>
       </c>
       <c r="F32" s="57" t="s">
         <v>77</v>
@@ -6088,7 +6088,7 @@
         <v>94</v>
       </c>
       <c r="H32" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I32" s="21" t="s">
         <v>103</v>
@@ -6109,7 +6109,7 @@
       <c r="S32" s="63"/>
       <c r="T32" s="157"/>
       <c r="U32" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V32">
         <v>90</v>
@@ -6124,7 +6124,7 @@
     </row>
     <row r="33" spans="1:29" s="160" customFormat="1" ht="25" customHeight="1">
       <c r="A33" s="40" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B33" s="56" t="s">
         <v>37</v>
@@ -6136,7 +6136,7 @@
         <v>290</v>
       </c>
       <c r="E33" s="58" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="F33" s="57" t="s">
         <v>77</v>
@@ -6145,7 +6145,7 @@
         <v>94</v>
       </c>
       <c r="H33" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I33" s="21" t="s">
         <v>103</v>
@@ -6166,7 +6166,7 @@
       <c r="S33" s="63"/>
       <c r="T33" s="157"/>
       <c r="U33" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V33">
         <v>95</v>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="34" spans="1:29" s="160" customFormat="1" ht="25" customHeight="1">
       <c r="A34" s="40" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B34" s="56" t="s">
         <v>37</v>
@@ -6193,7 +6193,7 @@
         <v>290</v>
       </c>
       <c r="E34" s="58" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="F34" s="57" t="s">
         <v>77</v>
@@ -6202,7 +6202,7 @@
         <v>94</v>
       </c>
       <c r="H34" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I34" s="21" t="s">
         <v>103</v>
@@ -6223,7 +6223,7 @@
       <c r="S34" s="63"/>
       <c r="T34" s="157"/>
       <c r="U34" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="V34">
         <v>100</v>
@@ -6257,8 +6257,8 @@
       <c r="R35" s="62"/>
       <c r="S35" s="63"/>
       <c r="T35" s="157"/>
-      <c r="U35"/>
-      <c r="V35"/>
+      <c r="U35" s="171"/>
+      <c r="V35" s="64"/>
       <c r="W35" s="158"/>
       <c r="X35" s="65"/>
       <c r="Y35" s="65"/>
@@ -6288,8 +6288,8 @@
       <c r="R36" s="62"/>
       <c r="S36" s="63"/>
       <c r="T36" s="157"/>
-      <c r="U36"/>
-      <c r="V36"/>
+      <c r="U36" s="171"/>
+      <c r="V36" s="64"/>
       <c r="W36" s="158"/>
       <c r="X36" s="65"/>
       <c r="Y36" s="65"/>
@@ -6319,8 +6319,8 @@
       <c r="R37" s="62"/>
       <c r="S37" s="63"/>
       <c r="T37" s="157"/>
-      <c r="U37"/>
-      <c r="V37"/>
+      <c r="U37" s="171"/>
+      <c r="V37" s="64"/>
       <c r="W37" s="158"/>
       <c r="X37" s="65"/>
       <c r="Y37" s="65"/>
@@ -6350,8 +6350,8 @@
       <c r="R38" s="62"/>
       <c r="S38" s="63"/>
       <c r="T38" s="157"/>
-      <c r="U38"/>
-      <c r="V38"/>
+      <c r="U38" s="171"/>
+      <c r="V38" s="64"/>
       <c r="W38" s="158"/>
       <c r="X38" s="65"/>
       <c r="Y38" s="65"/>
@@ -6381,8 +6381,8 @@
       <c r="R39" s="62"/>
       <c r="S39" s="63"/>
       <c r="T39" s="157"/>
-      <c r="U39"/>
-      <c r="V39"/>
+      <c r="U39" s="171"/>
+      <c r="V39" s="64"/>
       <c r="W39" s="158"/>
       <c r="X39" s="65"/>
       <c r="Y39" s="65"/>
@@ -6412,8 +6412,8 @@
       <c r="R40" s="62"/>
       <c r="S40" s="63"/>
       <c r="T40" s="157"/>
-      <c r="U40"/>
-      <c r="V40"/>
+      <c r="U40" s="171"/>
+      <c r="V40" s="64"/>
       <c r="W40" s="158"/>
       <c r="X40" s="65"/>
       <c r="Y40" s="65"/>
@@ -6443,8 +6443,8 @@
       <c r="R41" s="62"/>
       <c r="S41" s="63"/>
       <c r="T41" s="157"/>
-      <c r="U41"/>
-      <c r="V41"/>
+      <c r="U41" s="171"/>
+      <c r="V41" s="64"/>
       <c r="W41" s="158"/>
       <c r="X41" s="65"/>
       <c r="Y41" s="65"/>
@@ -6474,8 +6474,8 @@
       <c r="R42" s="62"/>
       <c r="S42" s="63"/>
       <c r="T42" s="157"/>
-      <c r="U42"/>
-      <c r="V42"/>
+      <c r="U42" s="171"/>
+      <c r="V42" s="64"/>
       <c r="W42" s="158"/>
       <c r="X42" s="65"/>
       <c r="Y42" s="65"/>
@@ -6505,8 +6505,8 @@
       <c r="R43" s="62"/>
       <c r="S43" s="63"/>
       <c r="T43" s="157"/>
-      <c r="U43"/>
-      <c r="V43"/>
+      <c r="U43" s="171"/>
+      <c r="V43" s="64"/>
       <c r="W43" s="158"/>
       <c r="X43" s="65"/>
       <c r="Y43" s="65"/>
@@ -6536,8 +6536,8 @@
       <c r="R44" s="62"/>
       <c r="S44" s="63"/>
       <c r="T44" s="157"/>
-      <c r="U44"/>
-      <c r="V44"/>
+      <c r="U44" s="171"/>
+      <c r="V44" s="64"/>
       <c r="W44" s="158"/>
       <c r="X44" s="65"/>
       <c r="Y44" s="65"/>
@@ -6567,8 +6567,8 @@
       <c r="R45" s="62"/>
       <c r="S45" s="63"/>
       <c r="T45" s="157"/>
-      <c r="U45"/>
-      <c r="V45"/>
+      <c r="U45" s="171"/>
+      <c r="V45" s="64"/>
       <c r="W45" s="158"/>
       <c r="X45" s="65"/>
       <c r="Y45" s="65"/>
@@ -6598,8 +6598,8 @@
       <c r="R46" s="62"/>
       <c r="S46" s="63"/>
       <c r="T46" s="157"/>
-      <c r="U46"/>
-      <c r="V46"/>
+      <c r="U46" s="171"/>
+      <c r="V46" s="64"/>
       <c r="W46" s="158"/>
       <c r="X46" s="65"/>
       <c r="Y46" s="65"/>
@@ -6629,8 +6629,8 @@
       <c r="R47" s="62"/>
       <c r="S47" s="63"/>
       <c r="T47" s="157"/>
-      <c r="U47"/>
-      <c r="V47"/>
+      <c r="U47" s="171"/>
+      <c r="V47" s="64"/>
       <c r="W47" s="158"/>
       <c r="X47" s="65"/>
       <c r="Y47" s="65"/>
@@ -6660,8 +6660,8 @@
       <c r="R48" s="62"/>
       <c r="S48" s="63"/>
       <c r="T48" s="157"/>
-      <c r="U48"/>
-      <c r="V48"/>
+      <c r="U48" s="171"/>
+      <c r="V48" s="64"/>
       <c r="W48" s="158"/>
       <c r="X48" s="65"/>
       <c r="Y48" s="65"/>
@@ -6691,8 +6691,8 @@
       <c r="R49" s="62"/>
       <c r="S49" s="63"/>
       <c r="T49" s="157"/>
-      <c r="U49"/>
-      <c r="V49"/>
+      <c r="U49" s="171"/>
+      <c r="V49" s="64"/>
       <c r="W49" s="158"/>
       <c r="X49" s="65"/>
       <c r="Y49" s="65"/>
@@ -6722,8 +6722,8 @@
       <c r="R50" s="62"/>
       <c r="S50" s="63"/>
       <c r="T50" s="157"/>
-      <c r="U50"/>
-      <c r="V50"/>
+      <c r="U50" s="171"/>
+      <c r="V50" s="64"/>
       <c r="W50" s="158"/>
       <c r="X50" s="65"/>
       <c r="Y50" s="65"/>
@@ -6753,8 +6753,8 @@
       <c r="R51" s="62"/>
       <c r="S51" s="63"/>
       <c r="T51" s="157"/>
-      <c r="U51"/>
-      <c r="V51"/>
+      <c r="U51" s="171"/>
+      <c r="V51" s="64"/>
       <c r="W51" s="158"/>
       <c r="X51" s="65"/>
       <c r="Y51" s="65"/>
@@ -6784,8 +6784,8 @@
       <c r="R52" s="62"/>
       <c r="S52" s="63"/>
       <c r="T52" s="157"/>
-      <c r="U52"/>
-      <c r="V52"/>
+      <c r="U52" s="171"/>
+      <c r="V52" s="64"/>
       <c r="W52" s="158"/>
       <c r="X52" s="65"/>
       <c r="Y52" s="65"/>
@@ -6815,8 +6815,8 @@
       <c r="R53" s="62"/>
       <c r="S53" s="63"/>
       <c r="T53" s="157"/>
-      <c r="U53"/>
-      <c r="V53"/>
+      <c r="U53" s="171"/>
+      <c r="V53" s="64"/>
       <c r="W53" s="158"/>
       <c r="X53" s="65"/>
       <c r="Y53" s="65"/>
@@ -6846,8 +6846,8 @@
       <c r="R54" s="62"/>
       <c r="S54" s="63"/>
       <c r="T54" s="157"/>
-      <c r="U54"/>
-      <c r="V54"/>
+      <c r="U54" s="171"/>
+      <c r="V54" s="64"/>
       <c r="W54" s="158"/>
       <c r="X54" s="65"/>
       <c r="Y54" s="65"/>
@@ -6877,8 +6877,8 @@
       <c r="R55" s="62"/>
       <c r="S55" s="63"/>
       <c r="T55" s="157"/>
-      <c r="U55"/>
-      <c r="V55"/>
+      <c r="U55" s="171"/>
+      <c r="V55" s="64"/>
       <c r="W55" s="158"/>
       <c r="X55" s="65"/>
       <c r="Y55" s="65"/>
@@ -6908,8 +6908,8 @@
       <c r="R56" s="62"/>
       <c r="S56" s="63"/>
       <c r="T56" s="157"/>
-      <c r="U56"/>
-      <c r="V56"/>
+      <c r="U56" s="171"/>
+      <c r="V56" s="64"/>
       <c r="W56" s="158"/>
       <c r="X56" s="65"/>
       <c r="Y56" s="65"/>
@@ -6939,8 +6939,8 @@
       <c r="R57" s="62"/>
       <c r="S57" s="63"/>
       <c r="T57" s="157"/>
-      <c r="U57"/>
-      <c r="V57"/>
+      <c r="U57" s="171"/>
+      <c r="V57" s="64"/>
       <c r="W57" s="158"/>
       <c r="X57" s="65"/>
       <c r="Y57" s="65"/>
@@ -6970,8 +6970,8 @@
       <c r="R58" s="62"/>
       <c r="S58" s="63"/>
       <c r="T58" s="157"/>
-      <c r="U58"/>
-      <c r="V58"/>
+      <c r="U58" s="171"/>
+      <c r="V58" s="64"/>
       <c r="W58" s="158"/>
       <c r="X58" s="65"/>
       <c r="Y58" s="65"/>
@@ -7001,8 +7001,8 @@
       <c r="R59" s="62"/>
       <c r="S59" s="63"/>
       <c r="T59" s="157"/>
-      <c r="U59"/>
-      <c r="V59"/>
+      <c r="U59" s="171"/>
+      <c r="V59" s="64"/>
       <c r="W59" s="158"/>
       <c r="X59" s="65"/>
       <c r="Y59" s="65"/>
@@ -7032,8 +7032,8 @@
       <c r="R60" s="62"/>
       <c r="S60" s="63"/>
       <c r="T60" s="157"/>
-      <c r="U60"/>
-      <c r="V60"/>
+      <c r="U60" s="171"/>
+      <c r="V60" s="64"/>
       <c r="W60" s="158"/>
       <c r="X60" s="65"/>
       <c r="Y60" s="65"/>
@@ -7063,8 +7063,8 @@
       <c r="R61" s="62"/>
       <c r="S61" s="63"/>
       <c r="T61" s="157"/>
-      <c r="U61"/>
-      <c r="V61"/>
+      <c r="U61" s="171"/>
+      <c r="V61" s="64"/>
       <c r="W61" s="158"/>
       <c r="X61" s="65"/>
       <c r="Y61" s="65"/>
@@ -7094,8 +7094,8 @@
       <c r="R62" s="62"/>
       <c r="S62" s="63"/>
       <c r="T62" s="157"/>
-      <c r="U62"/>
-      <c r="V62"/>
+      <c r="U62" s="171"/>
+      <c r="V62" s="64"/>
       <c r="W62" s="158"/>
       <c r="X62" s="65"/>
       <c r="Y62" s="65"/>
@@ -7125,8 +7125,8 @@
       <c r="R63" s="62"/>
       <c r="S63" s="63"/>
       <c r="T63" s="157"/>
-      <c r="U63"/>
-      <c r="V63"/>
+      <c r="U63" s="171"/>
+      <c r="V63" s="64"/>
       <c r="W63" s="158"/>
       <c r="X63" s="65"/>
       <c r="Y63" s="65"/>
@@ -7156,8 +7156,8 @@
       <c r="R64" s="62"/>
       <c r="S64" s="63"/>
       <c r="T64" s="157"/>
-      <c r="U64"/>
-      <c r="V64"/>
+      <c r="U64" s="171"/>
+      <c r="V64" s="64"/>
       <c r="W64" s="158"/>
       <c r="X64" s="65"/>
       <c r="Y64" s="65"/>
@@ -7187,8 +7187,8 @@
       <c r="R65" s="62"/>
       <c r="S65" s="63"/>
       <c r="T65" s="157"/>
-      <c r="U65"/>
-      <c r="V65"/>
+      <c r="U65" s="171"/>
+      <c r="V65" s="64"/>
       <c r="W65" s="158"/>
       <c r="X65" s="65"/>
       <c r="Y65" s="65"/>
@@ -7218,8 +7218,8 @@
       <c r="R66" s="62"/>
       <c r="S66" s="63"/>
       <c r="T66" s="157"/>
-      <c r="U66"/>
-      <c r="V66"/>
+      <c r="U66" s="171"/>
+      <c r="V66" s="64"/>
       <c r="W66" s="158"/>
       <c r="X66" s="65"/>
       <c r="Y66" s="65"/>
@@ -17610,11 +17610,11 @@
     <mergeCell ref="U9:V9"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L15:L394" xr:uid="{8D7FB32C-3427-2549-AEE5-4D4BF06D9402}">
       <formula1>#REF!</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K15:K394" xr:uid="{1590E11D-D86A-FC45-B310-31384307009E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K15:K66" xr:uid="{F3A51455-22C1-C340-91E0-3A9F0363D218}">
       <formula1>$I$3:$I$7</formula1>
     </dataValidation>
   </dataValidations>
@@ -17629,96 +17629,198 @@
   <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="15">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="32">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{3D101648-861B-C44F-9EA1-C1DFE8FE106F}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$E$3:$E$103</xm:f>
           </x14:formula1>
-          <xm:sqref>B15:B394</xm:sqref>
+          <xm:sqref>B67:B394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C94ACB21-8575-E349-97C4-9188D8686827}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$D$3:$D$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F15:F394</xm:sqref>
+          <xm:sqref>F67:F394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7604AA96-D86E-8C49-95DF-A8C3A1F9AA6D}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$K$3:$K$98</xm:f>
           </x14:formula1>
-          <xm:sqref>N15:N394</xm:sqref>
+          <xm:sqref>N67:N394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0D030033-729E-3940-A2F0-6EDE030A4235}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$A$3:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K15:K394</xm:sqref>
+          <xm:sqref>K67:K394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0AB04B6F-DD6D-D24E-8CD7-22596E657E09}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$M$3:$M$102</xm:f>
           </x14:formula1>
-          <xm:sqref>W15:W394</xm:sqref>
+          <xm:sqref>W67:W394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F8862D0-5953-E940-A175-C24E85C556BA}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$H$3:$H$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G15:G394</xm:sqref>
+          <xm:sqref>G67:G394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{049A1BE4-E9DE-0D4B-868D-02E76474AFA5}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$J$3:$J$5</xm:f>
           </x14:formula1>
-          <xm:sqref>Q15:Q394</xm:sqref>
+          <xm:sqref>Q67:Q394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{08D5E3A7-E133-A54A-8435-B3FB6647D742}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$B$3:$B$6</xm:f>
           </x14:formula1>
-          <xm:sqref>C15:C394</xm:sqref>
+          <xm:sqref>C67:C394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{BEC08EC3-9F4B-6843-8C63-E99D96F3B80C}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$I$3:$I$7</xm:f>
           </x14:formula1>
-          <xm:sqref>I15:I394</xm:sqref>
+          <xm:sqref>I67:I394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B9CE73CA-32E5-CD40-909B-B3388F139783}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$M$3:$M$22</xm:f>
           </x14:formula1>
-          <xm:sqref>V15:V394</xm:sqref>
+          <xm:sqref>V67:V394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{AE62419B-1860-B240-A67A-B0DC077CD735}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$N$3:$N$4</xm:f>
           </x14:formula1>
-          <xm:sqref>Z15:Z394</xm:sqref>
+          <xm:sqref>Z67:Z394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{69271FA2-0E38-394D-9669-1C78E1B7E49C}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$F$3:$F$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G15:G394 J15:K394</xm:sqref>
+          <xm:sqref>G67:G394 J67:K394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{7180FD00-41DF-8643-B71E-0C3BEC5EA22D}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$L$3:$L$54</xm:f>
           </x14:formula1>
-          <xm:sqref>P15:P394</xm:sqref>
+          <xm:sqref>P67:P394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{420DCC94-8F2C-ED4B-99EB-812BBC021162}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$C$3:$C$24</xm:f>
           </x14:formula1>
-          <xm:sqref>D15:D394</xm:sqref>
+          <xm:sqref>D67:D394</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88BF134A-5ECF-2B44-AD8A-3C294F943CA6}">
           <x14:formula1>
             <xm:f>'Drop down lists'!$G$3:$G$13</xm:f>
           </x14:formula1>
-          <xm:sqref>H15:H394 K15:K394</xm:sqref>
+          <xm:sqref>H67:H394 K67:K394</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F7E859BE-ACD8-0B41-ACC2-676CE139802B}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B35:C66 V35:W66 Z35:Z66 F35:K66 P35:Q66 N35:N66</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{D7269B74-18FD-E641-B429-B50E3A0E073A}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D35:D66</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{029CF89E-9F0F-3944-A529-A257592A3730}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>H15:H34 K15:K34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Make sure the information matches the valid Application tags in the information tab" xr:uid="{1360AB10-48F2-334D-8C59-3C2A0AC11A9E}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>D15:D34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{32F4E395-6F5E-1940-8CAE-094B06F4652C}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>P15:P34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{444349C7-3296-E447-97C1-9B2685A07ED4}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G15:G34 J15:K34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9690FD5F-8EC8-B34D-BB73-0E43A1D6BDDC}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>Z15:Z34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{577A7963-29CF-3449-B60E-55584428E89A}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>V15:V34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ED4BF276-CC93-DE46-9B22-1176664A0AB4}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>I15:I34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{978E96B5-8B99-EA45-A783-57648647A9C3}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>C15:C34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2A7C75C9-EDB9-9E4F-81FB-CE82D3E84A9F}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>Q15:Q34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C57AC945-A5FC-8E47-BCF1-6EF95AF413BF}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G15:G34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{0434F97A-F4E5-AE49-9657-E999EDDA02DF}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>W15:W34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EDF3E33E-A3F7-7D49-BF29-5F485944482B}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>K15:K34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{88297A13-23C2-B646-B139-614C3ED2CB68}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>N15:N34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{933E1487-7298-4745-9C19-921867A52EF8}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F15:F34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{17CC1280-BF95-3347-BF63-64933195F117}">
+          <x14:formula1>
+            <xm:f>'Drop down lists'!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>B15:B34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -17734,7 +17836,7 @@
   <dimension ref="A1:AK103"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3:M22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -17809,7 +17911,7 @@
         <v>253</v>
       </c>
       <c r="N2" s="55" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="O2" s="44"/>
       <c r="P2" s="43"/>
@@ -17840,7 +17942,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="38" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C3" s="30" t="s">
         <v>288</v>
@@ -17876,7 +17978,7 @@
         <v>5</v>
       </c>
       <c r="N3" s="31" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="O3" s="22"/>
       <c r="P3" s="22"/>
@@ -17927,7 +18029,7 @@
         <v>10</v>
       </c>
       <c r="N4" s="31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="O4" s="22"/>
       <c r="P4" s="22"/>
@@ -17983,7 +18085,7 @@
     <row r="6" spans="1:37">
       <c r="A6" s="32"/>
       <c r="B6" s="38" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>291</v>
@@ -18028,10 +18130,10 @@
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="42" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="I7" s="176" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K7" s="175" t="s">
         <v>31</v>
@@ -18201,7 +18303,7 @@
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="176" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
@@ -18236,7 +18338,7 @@
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="176" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
@@ -18263,7 +18365,7 @@
       <c r="A14" s="32"/>
       <c r="B14" s="33"/>
       <c r="C14" s="30" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="21" t="s">
@@ -18313,7 +18415,7 @@
         <v>117</v>
       </c>
       <c r="L15" s="172" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M15">
         <v>65</v>
@@ -18331,7 +18433,7 @@
       <c r="A16" s="32"/>
       <c r="B16" s="34"/>
       <c r="C16" s="30" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D16" s="22"/>
       <c r="E16" s="21" t="s">
@@ -18364,7 +18466,7 @@
       <c r="A17" s="32"/>
       <c r="B17" s="34"/>
       <c r="C17" s="53" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="D17" s="22"/>
       <c r="E17" s="21" t="s">
@@ -18430,7 +18532,7 @@
       <c r="A19" s="32"/>
       <c r="B19" s="34"/>
       <c r="C19" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="21" t="s">
@@ -18496,7 +18598,7 @@
       <c r="A21" s="32"/>
       <c r="B21" s="34"/>
       <c r="C21" s="30" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="21" t="s">
@@ -18544,7 +18646,7 @@
         <v>110</v>
       </c>
       <c r="L22" s="172" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M22">
         <v>100</v>
@@ -18607,7 +18709,7 @@
         <v>112</v>
       </c>
       <c r="L24" s="31" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
@@ -18715,7 +18817,7 @@
         <v>131</v>
       </c>
       <c r="L28" s="172" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="N28" s="22"/>
       <c r="O28" s="22"/>
@@ -18882,7 +18984,7 @@
         <v>185</v>
       </c>
       <c r="L34" s="172" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="N34" s="22"/>
       <c r="O34" s="22"/>
@@ -20640,6 +20742,7 @@
       <c r="U103" s="22"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="AlryAM3vCnGy9MjXjTugKlzYaBLXZjLFYA9egPMQNhCW9Rq5MHQApudHrT0cbI+iO4Nvz6A4Rff9jagAqBw+Hw==" saltValue="r2WjgYLC3iN7hYZov2+P2A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <sortState ref="L3:L44">
     <sortCondition ref="L44"/>
   </sortState>

</xml_diff>